<commit_message>
Pushing Changes Added Sample test to launch application and login
</commit_message>
<xml_diff>
--- a/coxaxle/src/test/resources/datasheets/SampleTest.xlsx
+++ b/coxaxle/src/test/resources/datasheets/SampleTest.xlsx
@@ -15,18 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Role</t>
+    <t>Email</t>
   </si>
   <si>
-    <t>REQUESTOR</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>XEEVA -MJ</t>
+    <t>email_1</t>
   </si>
 </sst>
 </file>
@@ -558,8 +552,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -856,39 +878,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>